<commit_message>
[MS-AUTHWS]: Update RS according to lastest version TD
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\InteropO15Dev\TestSuites\SharePoint\Platinum\SPSPTS_Dev\SharePoint Server Protocol Test Suites\Docs\MS-AUTHWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-AUTHWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$143</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$145</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="342">
   <si>
     <t>Req ID</t>
   </si>
@@ -541,9 +541,6 @@
     <t>MS-AUTHWS_R57</t>
   </si>
   <si>
-    <t>MS-AUTHWS_R58</t>
-  </si>
-  <si>
     <t>MS-AUTHWS_R59</t>
   </si>
   <si>
@@ -673,9 +670,6 @@
     <t>MS-AUTHWS_R95</t>
   </si>
   <si>
-    <t>MS-AUTHWS_R96</t>
-  </si>
-  <si>
     <t>MS-AUTHWS_R97</t>
   </si>
   <si>
@@ -962,12 +956,6 @@
   </si>
   <si>
     <t>[In Message Processing Events and Sequencing Rules] The operation "Login" logs a user onto an application by using the user’s logon name and password.</t>
-  </si>
-  <si>
-    <t>[In Message Processing Events and Sequencing Rules] The operation "Mode" retrieves the authentication mode that a Web application (1) uses.</t>
-  </si>
-  <si>
-    <t>[In Login] The Login operation logs a user onto a Web application (1) by using the user’s logon name and password.</t>
   </si>
   <si>
     <t>[In Login] For the operation [Login operation] to succeed, the protocol server MUST use forms authentication and the logon name and password that is provided by the protocol client MUST be valid.</t>
@@ -1011,9 +999,6 @@
   </si>
   <si>
     <t>[In LoginSoapOut] The LoginSoapOut message is the response WSDL message that is used by a protocol server when logging on a user in response to a LoginSoapIn request message.</t>
-  </si>
-  <si>
-    <t>[In LoginSoapOut] The SOAP action value of the message [LoginSoapOut message] is defined as [follows]: http://schemas.microsoft.com/sharepoint/soap/Login</t>
   </si>
   <si>
     <t>[In LoginSoapOut] The SOAP body contains a LoginResponse element, as specified in section 3.1.4.1.2.2.</t>
@@ -1089,9 +1074,6 @@
     <t>[In LoginResult] ErrorCode: An error code, as specified in section 3.1.4.1.4.1.</t>
   </si>
   <si>
-    <t>[In LoginResult] TimeoutSeconds: An integer that specifies the number of seconds before the cookie, which is specified in the CookieName element, expires.</t>
-  </si>
-  <si>
     <t>[In Simple Types] The following XML Schema simple type definitions are specific to this operation.</t>
   </si>
   <si>
@@ -1135,21 +1117,6 @@
     <t>[In LoginErrorCode] The value of LoginErrorCode is "PasswordNotMatch", the Login operation failed because the password does not match what is stored on the server.</t>
   </si>
   <si>
-    <t>[In Mode] The Mode operation retrieves the authentication mode that a Web application (1) uses.</t>
-  </si>
-  <si>
-    <t>[In Mode] The Mode operation retrieves the authentication mode [Forms] that a Web application (1) uses.</t>
-  </si>
-  <si>
-    <t>[In Mode] The Mode operation retrieves the authentication mode [None] that a Web application (1) uses.</t>
-  </si>
-  <si>
-    <t>[In Mode] The Mode operation retrieves the authentication mode [Windows] that a Web application (1) uses.</t>
-  </si>
-  <si>
-    <t>[In Mode] The Mode operation retrieves the authentication mode [Passport] that a Web application (1) uses.</t>
-  </si>
-  <si>
     <t>[In Mode] [The Mode operation is defined as follows:]
 &lt;wsdl:operation name="Mode"&gt;
     &lt;wsdl:input message="tns:ModeSoapIn" /&gt;
@@ -1174,10 +1141,6 @@
   </si>
   <si>
     <t>[In ModeSoapOut] The ModeSoapOut message is the response WSDL message that a protocol server sends after retrieving the authentication mode.</t>
-  </si>
-  <si>
-    <t>[In ModeSoapOut] The SOAP action value of the message [ModeSoapOut message] is defined as:
-http://schemas.microsoft.com/sharepoint/soap/Mode</t>
   </si>
   <si>
     <t>[In ModeSoapOut] The SOAP body contains a ModeResponse element, as specified in section 3.1.4.2.2.2.</t>
@@ -1206,9 +1169,6 @@
   </si>
   <si>
     <t>[In ModeResponse] ModeResult: An AuthenticationMode simple type, as specified in section 3.1.4.2.4.1.</t>
-  </si>
-  <si>
-    <t>[In AuthenticationMode] The AuthenticationMode simple type specifies the authentication mode for the Login WSDL operation.</t>
   </si>
   <si>
     <t>[In AuthenticationMode] [The AuthenticationMode simple type is defined as follows:]
@@ -1225,21 +1185,12 @@
     <t>[In AuthenticationMode] The AuthenticationMode field has four allowable values:  [None, Windows, Passport, Forms].</t>
   </si>
   <si>
-    <t>[In AuthenticationMode] If the AuthenticationMode is "None", no authentication is used [or a custom authentication scheme is used].</t>
-  </si>
-  <si>
-    <t>[In AuthenticationMode] If the AuthenticationMode is "None", a custom authentication scheme is used.</t>
-  </si>
-  <si>
     <t>[In AuthenticationMode] If the AuthenticationMode is "Windows", authentication is handled by Internet Information Services (IIS).</t>
   </si>
   <si>
     <t>[In AuthenticationMode] If the AuthenticationMode is "Windows" [authentication is handled by IIS], the application context uses a security token that is received from IIS.</t>
   </si>
   <si>
-    <t>[In AuthenticationMode] If the AuthenticationMode is "Passport&lt;2&gt;", Windows Live ID is used for authentication.</t>
-  </si>
-  <si>
     <t>[In AuthenticationMode] If the AuthenticationMode is "Forms", a protocol client submits credentials by using an HTML form.</t>
   </si>
   <si>
@@ -1253,9 +1204,6 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Unless otherwise specified, the term MAY implies that the product does not follow the prescription.</t>
-  </si>
-  <si>
-    <t>[In Appendix B: Product Behavior] &lt;2&gt; Section 3.1.4.2.4.1: Use of Windows Live ID for authentication is not supported by Windows Server 2008.</t>
   </si>
   <si>
     <t>MS-AUTHWS_R3:c</t>
@@ -1302,24 +1250,99 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Implementation does return the default value of the CookieName which is "FedAuth".(The Microsoft SharePoint Foundation 2010 and Microsoft SharePoint Foundation 2013 follow this behavior.)</t>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior] Implementation does return the default value of the CookieName which is ".ASPXAUTH". &lt;1&gt; Section 3.1.4.1.3.1:  Windows SharePoint Services 3.0 returns the default value of ".ASPXAUTH".</t>
   </si>
   <si>
     <t>Open Specification Date:</t>
+  </si>
+  <si>
+    <t>[In Message Processing Events and Sequencing Rules] The operation "Mode" retrieves the authentication mode that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In Login] The Login operation logs a user onto a Web application by using the user’s logon name and password.</t>
+  </si>
+  <si>
+    <t>[In Mode] The Mode operation retrieves the authentication mode that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In Mode] The Mode operation retrieves the authentication mode [Forms] that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In Mode] The Mode operation retrieves the authentication mode [None] that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In Mode] The Mode operation retrieves the authentication mode [Windows] that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In Mode] The Mode operation retrieves the authentication mode [Passport] that a Web application uses.</t>
+  </si>
+  <si>
+    <t>[In LoginResult] TimeoutSeconds: An integer that specifies the number of seconds before the cookie, which is specified in the CookieName element, expires. &lt;2&gt;</t>
+  </si>
+  <si>
+    <t>[In AuthenticationMode] The AuthenticationMode simple type specifies the authentication mode for the Mode WSDL operation.</t>
+  </si>
+  <si>
+    <t>[In AuthenticationMode] If the AuthenticationMode is "None"&lt;3&gt;, no authentication is used [or a custom authentication scheme is used].</t>
+  </si>
+  <si>
+    <t>[In AuthenticationMode] If the AuthenticationMode is "None"&lt;3&gt;, a custom authentication scheme is used.</t>
+  </si>
+  <si>
+    <t>[In AuthenticationMode] If the AuthenticationMode is "Passport&lt;4&gt;", Windows Live ID is used for authentication.</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does return the default value of the CookieName which is "FedAuth".(The Microsoft SharePoint Foundation 2010, Microsoft SharePoint Foundation 2013 and Microsoft SharePoint Server 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R190</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R191</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R192</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R193</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R76:i</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does not return the element TimeoutSeconds. (&lt;2&gt; Section 3.1.4.1.3.1:  Windows SharePoint Services 3.0 does not return this element.)</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does return the element TimeoutSeconds that specifies the number of seconds before the cookie, which is specified in the CookieName element, expires. (The Microsoft SharePoint Foundation 2010, Microsoft SharePoint Foundation 2013 and Microsoft SharePoint Server 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R115:i</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does return "Forms" when the value for AuthenticationMode is "None". (&lt;3&gt; Section 3.1.4.2.4.1:  Microsoft SharePoint Foundation 2010 Service Pack 1 returns "Forms" when the value for AuthenticationMode is "None".)</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Implementation does not use authentication if the AuthenticationMode is "None". (Windows SharePoint Services 3.0, Microsoft SharePoint Foundation 2013 and Microsoft SharePoint Server 2016 follow this behavior.)</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-AUTHWS_R190,MS-AUTHWS_R191.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-AUTHWS_R192,MS-AUTHWS_R193.</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] &lt;4&gt; Section 3.1.4.2.4.1: Use of Windows Live ID for authentication is not supported by Windows Server 2008 operating system with Service Pack 2 (SP2) and Windows Server 2012 operating system.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1364,6 +1387,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1511,7 +1539,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1581,20 +1609,8 @@
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1620,11 +1636,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="27">
     <dxf>
       <font>
         <b val="0"/>
@@ -1964,36 +1995,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.59996337778862885"/>
@@ -2166,8 +2167,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I143" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I143"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I145" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I145"/>
   <tableColumns count="9">
     <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -2289,6 +2290,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2324,6 +2342,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2501,28 +2536,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:L147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>327</v>
+        <v>310</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2532,7 +2567,7 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>328</v>
+        <v>311</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2546,138 +2581,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>3.1</v>
+        <v>4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="F3" s="12">
-        <v>41481</v>
+        <v>42566</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="46"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="34" t="s">
+      <c r="B7" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
+      <c r="C8" s="43"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
+      <c r="H8" s="43"/>
+      <c r="I8" s="43"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="38"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="34"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2690,12 +2725,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
+      <c r="F12" s="35"/>
+      <c r="G12" s="35"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2708,12 +2743,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
+      <c r="H13" s="36"/>
+      <c r="I13" s="36"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2726,12 +2761,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2744,60 +2779,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="41"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="45"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2836,10 +2871,10 @@
         <v>42</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22" t="s">
@@ -2856,15 +2891,15 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D21" s="22"/>
       <c r="E21" s="22" t="s">
@@ -2880,7 +2915,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>324</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" ht="30">
@@ -2888,10 +2923,10 @@
         <v>44</v>
       </c>
       <c r="B22" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22" t="s">
@@ -2913,13 +2948,13 @@
         <v>45</v>
       </c>
       <c r="B23" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>19</v>
@@ -2940,13 +2975,13 @@
         <v>46</v>
       </c>
       <c r="B24" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>317</v>
+        <v>300</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>19</v>
@@ -2967,10 +3002,10 @@
         <v>47</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22" t="s">
@@ -2992,10 +3027,10 @@
         <v>48</v>
       </c>
       <c r="B26" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D26" s="22"/>
       <c r="E26" s="22" t="s">
@@ -3012,15 +3047,15 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1">
       <c r="A27" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B27" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C27" s="20" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22" t="s">
@@ -3042,10 +3077,10 @@
         <v>50</v>
       </c>
       <c r="B28" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C28" s="20" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22" t="s">
@@ -3067,10 +3102,10 @@
         <v>51</v>
       </c>
       <c r="B29" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C29" s="20" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22" t="s">
@@ -3092,10 +3127,10 @@
         <v>52</v>
       </c>
       <c r="B30" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" s="20" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D30" s="22"/>
       <c r="E30" s="22" t="s">
@@ -3117,10 +3152,10 @@
         <v>53</v>
       </c>
       <c r="B31" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C31" s="20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D31" s="22"/>
       <c r="E31" s="22" t="s">
@@ -3137,15 +3172,15 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="32" spans="1:12" s="23" customFormat="1">
       <c r="A32" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B32" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C32" s="20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D32" s="22"/>
       <c r="E32" s="22" t="s">
@@ -3167,10 +3202,10 @@
         <v>55</v>
       </c>
       <c r="B33" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="22" t="s">
@@ -3187,15 +3222,15 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" ht="30">
+    <row r="34" spans="1:9">
       <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D34" s="30"/>
       <c r="E34" s="30" t="s">
@@ -3217,10 +3252,10 @@
         <v>57</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C35" s="32" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D35" s="30"/>
       <c r="E35" s="30" t="s">
@@ -3242,10 +3277,10 @@
         <v>58</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D36" s="30"/>
       <c r="E36" s="30" t="s">
@@ -3262,15 +3297,15 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="45">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30" t="s">
@@ -3287,15 +3322,15 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="45">
+    <row r="38" spans="1:9" ht="30">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30" t="s">
@@ -3317,10 +3352,10 @@
         <v>61</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D39" s="30"/>
       <c r="E39" s="30" t="s">
@@ -3337,15 +3372,15 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" ht="30">
+    <row r="40" spans="1:9">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D40" s="30"/>
       <c r="E40" s="30" t="s">
@@ -3367,10 +3402,10 @@
         <v>63</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D41" s="30"/>
       <c r="E41" s="30" t="s">
@@ -3392,10 +3427,10 @@
         <v>64</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D42" s="30"/>
       <c r="E42" s="30" t="s">
@@ -3412,15 +3447,15 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9">
       <c r="A43" s="30" t="s">
         <v>65</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D43" s="30"/>
       <c r="E43" s="30" t="s">
@@ -3437,15 +3472,15 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" ht="30">
+    <row r="44" spans="1:9">
       <c r="A44" s="30" t="s">
         <v>66</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C44" s="32" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D44" s="30"/>
       <c r="E44" s="30" t="s">
@@ -3462,15 +3497,15 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" ht="30">
+    <row r="45" spans="1:9">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C45" s="32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D45" s="30"/>
       <c r="E45" s="30" t="s">
@@ -3487,15 +3522,15 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" ht="30">
+    <row r="46" spans="1:9">
       <c r="A46" s="30" t="s">
         <v>68</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C46" s="32" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D46" s="30"/>
       <c r="E46" s="30" t="s">
@@ -3512,15 +3547,15 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" ht="30">
+    <row r="47" spans="1:9">
       <c r="A47" s="30" t="s">
         <v>69</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C47" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D47" s="30"/>
       <c r="E47" s="30" t="s">
@@ -3542,10 +3577,10 @@
         <v>70</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C48" s="32" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D48" s="30"/>
       <c r="E48" s="30" t="s">
@@ -3567,10 +3602,10 @@
         <v>71</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C49" s="32" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="D49" s="30"/>
       <c r="E49" s="30" t="s">
@@ -3592,10 +3627,10 @@
         <v>72</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C50" s="32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D50" s="30"/>
       <c r="E50" s="30" t="s">
@@ -3612,15 +3647,15 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" ht="30">
+    <row r="51" spans="1:9">
       <c r="A51" s="30" t="s">
         <v>73</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C51" s="32" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D51" s="30"/>
       <c r="E51" s="30" t="s">
@@ -3642,10 +3677,10 @@
         <v>74</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C52" s="32" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D52" s="30"/>
       <c r="E52" s="30" t="s">
@@ -3662,22 +3697,22 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="45">
+    <row r="53" spans="1:9" ht="30">
       <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C53" s="32" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D53" s="30"/>
       <c r="E53" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>329</v>
+        <v>312</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>15</v>
@@ -3692,10 +3727,10 @@
         <v>76</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C54" s="32" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="30" t="s">
@@ -3717,10 +3752,10 @@
         <v>77</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C55" s="32" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D55" s="30"/>
       <c r="E55" s="30" t="s">
@@ -3737,15 +3772,15 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="45">
+    <row r="56" spans="1:9" ht="30">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C56" s="32" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D56" s="30"/>
       <c r="E56" s="30" t="s">
@@ -3767,10 +3802,10 @@
         <v>79</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C57" s="32" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D57" s="30"/>
       <c r="E57" s="30" t="s">
@@ -3792,10 +3827,10 @@
         <v>80</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C58" s="32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D58" s="30"/>
       <c r="E58" s="30" t="s">
@@ -3817,10 +3852,10 @@
         <v>81</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C59" s="32" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D59" s="30"/>
       <c r="E59" s="30" t="s">
@@ -3842,10 +3877,10 @@
         <v>82</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>238</v>
+        <v>316</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -3870,7 +3905,7 @@
         <v>31</v>
       </c>
       <c r="C61" s="32" t="s">
-        <v>239</v>
+        <v>317</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
@@ -3887,7 +3922,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="45">
+    <row r="62" spans="1:9" ht="30">
       <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
@@ -3895,7 +3930,7 @@
         <v>31</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D62" s="30"/>
       <c r="E62" s="30" t="s">
@@ -3912,7 +3947,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="45">
+    <row r="63" spans="1:9" ht="30">
       <c r="A63" s="30" t="s">
         <v>85</v>
       </c>
@@ -3920,7 +3955,7 @@
         <v>31</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D63" s="30"/>
       <c r="E63" s="30" t="s">
@@ -3937,7 +3972,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="45">
+    <row r="64" spans="1:9" ht="30">
       <c r="A64" s="30" t="s">
         <v>86</v>
       </c>
@@ -3945,10 +3980,10 @@
         <v>31</v>
       </c>
       <c r="C64" s="32" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>19</v>
@@ -3972,10 +4007,10 @@
         <v>31</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
       <c r="E65" s="30" t="s">
         <v>19</v>
@@ -3991,7 +4026,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9">
       <c r="A66" s="30" t="s">
         <v>88</v>
       </c>
@@ -3999,7 +4034,7 @@
         <v>31</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D66" s="30"/>
       <c r="E66" s="30" t="s">
@@ -4024,7 +4059,7 @@
         <v>31</v>
       </c>
       <c r="C67" s="32" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D67" s="30"/>
       <c r="E67" s="30" t="s">
@@ -4049,7 +4084,7 @@
         <v>31</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="D68" s="30"/>
       <c r="E68" s="30" t="s">
@@ -4066,7 +4101,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="45">
+    <row r="69" spans="1:9" ht="30">
       <c r="A69" s="30" t="s">
         <v>91</v>
       </c>
@@ -4074,7 +4109,7 @@
         <v>31</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="D69" s="30"/>
       <c r="E69" s="30" t="s">
@@ -4096,10 +4131,10 @@
         <v>92</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C70" s="32" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="D70" s="30"/>
       <c r="E70" s="30" t="s">
@@ -4121,10 +4156,10 @@
         <v>93</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C71" s="32" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D71" s="30"/>
       <c r="E71" s="30" t="s">
@@ -4146,10 +4181,10 @@
         <v>94</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C72" s="32" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D72" s="30"/>
       <c r="E72" s="30" t="s">
@@ -4171,10 +4206,10 @@
         <v>95</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C73" s="32" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D73" s="30"/>
       <c r="E73" s="30" t="s">
@@ -4196,10 +4231,10 @@
         <v>96</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C74" s="32" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D74" s="30"/>
       <c r="E74" s="30" t="s">
@@ -4216,15 +4251,15 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" ht="30">
+    <row r="75" spans="1:9">
       <c r="A75" s="30" t="s">
         <v>97</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C75" s="32" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D75" s="30"/>
       <c r="E75" s="30" t="s">
@@ -4234,35 +4269,35 @@
         <v>6</v>
       </c>
       <c r="G75" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H75" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30">
+    <row r="76" spans="1:9">
       <c r="A76" s="30" t="s">
         <v>98</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C76" s="32" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="D76" s="30"/>
       <c r="E76" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F76" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G76" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H76" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I76" s="32"/>
     </row>
@@ -4271,17 +4306,17 @@
         <v>99</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C77" s="32" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D77" s="30"/>
       <c r="E77" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F77" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G77" s="30" t="s">
         <v>16</v>
@@ -4291,15 +4326,15 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9">
+    <row r="78" spans="1:9" ht="135">
       <c r="A78" s="30" t="s">
         <v>100</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C78" s="32" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D78" s="30"/>
       <c r="E78" s="30" t="s">
@@ -4309,22 +4344,22 @@
         <v>7</v>
       </c>
       <c r="G78" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H78" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" ht="135">
+    <row r="79" spans="1:9">
       <c r="A79" s="30" t="s">
         <v>101</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C79" s="32" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D79" s="30"/>
       <c r="E79" s="30" t="s">
@@ -4346,10 +4381,10 @@
         <v>102</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C80" s="32" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D80" s="30"/>
       <c r="E80" s="30" t="s">
@@ -4371,35 +4406,35 @@
         <v>103</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C81" s="32" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D81" s="30"/>
       <c r="E81" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F81" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G81" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H81" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="30">
+    <row r="82" spans="1:9" ht="120">
       <c r="A82" s="30" t="s">
         <v>104</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C82" s="32" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="D82" s="30"/>
       <c r="E82" s="30" t="s">
@@ -4409,22 +4444,22 @@
         <v>6</v>
       </c>
       <c r="G82" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H82" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" ht="120">
+    <row r="83" spans="1:9">
       <c r="A83" s="30" t="s">
         <v>105</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C83" s="32" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="D83" s="30"/>
       <c r="E83" s="30" t="s">
@@ -4441,15 +4476,15 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30">
+    <row r="84" spans="1:9">
       <c r="A84" s="30" t="s">
         <v>106</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C84" s="32" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D84" s="30"/>
       <c r="E84" s="30" t="s">
@@ -4459,22 +4494,22 @@
         <v>6</v>
       </c>
       <c r="G84" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H84" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I84" s="32"/>
     </row>
-    <row r="85" spans="1:9" ht="30">
+    <row r="85" spans="1:9">
       <c r="A85" s="30" t="s">
         <v>107</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C85" s="32" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D85" s="30"/>
       <c r="E85" s="30" t="s">
@@ -4484,10 +4519,10 @@
         <v>6</v>
       </c>
       <c r="G85" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H85" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I85" s="32"/>
     </row>
@@ -4496,10 +4531,10 @@
         <v>108</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C86" s="32" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D86" s="30"/>
       <c r="E86" s="30" t="s">
@@ -4512,19 +4547,19 @@
         <v>15</v>
       </c>
       <c r="H86" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="30">
+    <row r="87" spans="1:9" ht="120">
       <c r="A87" s="30" t="s">
         <v>109</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C87" s="32" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D87" s="30"/>
       <c r="E87" s="30" t="s">
@@ -4537,19 +4572,19 @@
         <v>15</v>
       </c>
       <c r="H87" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I87" s="32"/>
     </row>
-    <row r="88" spans="1:9" ht="120">
+    <row r="88" spans="1:9" ht="30">
       <c r="A88" s="30" t="s">
         <v>110</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C88" s="32" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="D88" s="30"/>
       <c r="E88" s="30" t="s">
@@ -4562,19 +4597,19 @@
         <v>15</v>
       </c>
       <c r="H88" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="30">
+    <row r="89" spans="1:9" ht="45">
       <c r="A89" s="30" t="s">
         <v>111</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C89" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="D89" s="30"/>
       <c r="E89" s="30" t="s">
@@ -4587,19 +4622,21 @@
         <v>15</v>
       </c>
       <c r="H89" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I89" s="32"/>
-    </row>
-    <row r="90" spans="1:9" ht="60">
+        <v>17</v>
+      </c>
+      <c r="I89" s="20" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="30" t="s">
         <v>112</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C90" s="32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D90" s="30"/>
       <c r="E90" s="30" t="s">
@@ -4612,21 +4649,19 @@
         <v>15</v>
       </c>
       <c r="H90" s="30" t="s">
-        <v>17</v>
-      </c>
-      <c r="I90" s="32" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" ht="30">
+        <v>20</v>
+      </c>
+      <c r="I90" s="32"/>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91" s="30" t="s">
         <v>113</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C91" s="32" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D91" s="30"/>
       <c r="E91" s="30" t="s">
@@ -4639,19 +4674,19 @@
         <v>15</v>
       </c>
       <c r="H91" s="30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9">
-      <c r="A92" s="30" t="s">
+    <row r="92" spans="1:9" ht="45">
+      <c r="A92" s="22" t="s">
         <v>114</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>186</v>
-      </c>
-      <c r="C92" s="32" t="s">
-        <v>270</v>
+        <v>184</v>
+      </c>
+      <c r="C92" s="20" t="s">
+        <v>323</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30" t="s">
@@ -4664,19 +4699,21 @@
         <v>15</v>
       </c>
       <c r="H92" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I92" s="32"/>
-    </row>
-    <row r="93" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I92" s="20" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93" s="30" t="s">
         <v>115</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C93" s="32" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D93" s="30"/>
       <c r="E93" s="30" t="s">
@@ -4686,22 +4723,22 @@
         <v>6</v>
       </c>
       <c r="G93" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H93" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" ht="30">
+    <row r="94" spans="1:9">
       <c r="A94" s="30" t="s">
         <v>116</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C94" s="32" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D94" s="30"/>
       <c r="E94" s="30" t="s">
@@ -4718,15 +4755,15 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="30">
+    <row r="95" spans="1:9" ht="120">
       <c r="A95" s="30" t="s">
         <v>117</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C95" s="32" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D95" s="30"/>
       <c r="E95" s="30" t="s">
@@ -4736,22 +4773,22 @@
         <v>6</v>
       </c>
       <c r="G95" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H95" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I95" s="32"/>
     </row>
-    <row r="96" spans="1:9" ht="120">
+    <row r="96" spans="1:9" ht="30">
       <c r="A96" s="30" t="s">
         <v>118</v>
       </c>
       <c r="B96" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C96" s="32" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D96" s="30"/>
       <c r="E96" s="30" t="s">
@@ -4773,10 +4810,10 @@
         <v>119</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C97" s="32" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D97" s="30"/>
       <c r="E97" s="30" t="s">
@@ -4789,7 +4826,7 @@
         <v>15</v>
       </c>
       <c r="H97" s="30" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I97" s="32"/>
     </row>
@@ -4798,10 +4835,10 @@
         <v>120</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C98" s="32" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D98" s="30"/>
       <c r="E98" s="30" t="s">
@@ -4818,17 +4855,19 @@
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="45">
+    <row r="99" spans="1:9" ht="30">
       <c r="A99" s="30" t="s">
         <v>121</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C99" s="32" t="s">
-        <v>277</v>
-      </c>
-      <c r="D99" s="30"/>
+        <v>272</v>
+      </c>
+      <c r="D99" s="30" t="s">
+        <v>302</v>
+      </c>
       <c r="E99" s="30" t="s">
         <v>19</v>
       </c>
@@ -4848,13 +4887,13 @@
         <v>122</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C100" s="32" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>19</v>
@@ -4875,13 +4914,13 @@
         <v>123</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C101" s="32" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>319</v>
+        <v>302</v>
       </c>
       <c r="E101" s="30" t="s">
         <v>19</v>
@@ -4893,23 +4932,23 @@
         <v>15</v>
       </c>
       <c r="H101" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I101" s="32"/>
+        <v>18</v>
+      </c>
+      <c r="I101" s="20" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="102" spans="1:9" ht="45">
       <c r="A102" s="30" t="s">
         <v>124</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C102" s="32" t="s">
-        <v>280</v>
-      </c>
-      <c r="D102" s="30" t="s">
-        <v>319</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
         <v>19</v>
       </c>
@@ -4920,23 +4959,23 @@
         <v>15</v>
       </c>
       <c r="H102" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I102" s="20" t="s">
-        <v>330</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="I102" s="32"/>
     </row>
     <row r="103" spans="1:9" ht="45">
       <c r="A103" s="30" t="s">
         <v>125</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>281</v>
-      </c>
-      <c r="D103" s="30"/>
+        <v>276</v>
+      </c>
+      <c r="D103" s="30" t="s">
+        <v>303</v>
+      </c>
       <c r="E103" s="30" t="s">
         <v>19</v>
       </c>
@@ -4951,18 +4990,18 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="45">
+    <row r="104" spans="1:9" ht="30">
       <c r="A104" s="30" t="s">
         <v>126</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>320</v>
+        <v>303</v>
       </c>
       <c r="E104" s="30" t="s">
         <v>19</v>
@@ -4978,24 +5017,22 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9">
       <c r="A105" s="30" t="s">
         <v>127</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>283</v>
-      </c>
-      <c r="D105" s="30" t="s">
-        <v>320</v>
-      </c>
+        <v>318</v>
+      </c>
+      <c r="D105" s="30"/>
       <c r="E105" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F105" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G105" s="30" t="s">
         <v>15</v>
@@ -5005,7 +5042,7 @@
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" ht="30">
+    <row r="106" spans="1:9">
       <c r="A106" s="30" t="s">
         <v>128</v>
       </c>
@@ -5013,9 +5050,11 @@
         <v>32</v>
       </c>
       <c r="C106" s="32" t="s">
-        <v>284</v>
-      </c>
-      <c r="D106" s="30"/>
+        <v>319</v>
+      </c>
+      <c r="D106" s="30" t="s">
+        <v>304</v>
+      </c>
       <c r="E106" s="30" t="s">
         <v>19</v>
       </c>
@@ -5030,7 +5069,7 @@
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" ht="30">
+    <row r="107" spans="1:9">
       <c r="A107" s="30" t="s">
         <v>129</v>
       </c>
@@ -5038,10 +5077,10 @@
         <v>32</v>
       </c>
       <c r="C107" s="32" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E107" s="30" t="s">
         <v>19</v>
@@ -5057,7 +5096,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" ht="30">
+    <row r="108" spans="1:9">
       <c r="A108" s="30" t="s">
         <v>130</v>
       </c>
@@ -5065,10 +5104,10 @@
         <v>32</v>
       </c>
       <c r="C108" s="32" t="s">
-        <v>286</v>
+        <v>321</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E108" s="30" t="s">
         <v>19</v>
@@ -5084,7 +5123,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" ht="30">
+    <row r="109" spans="1:9">
       <c r="A109" s="30" t="s">
         <v>131</v>
       </c>
@@ -5092,26 +5131,26 @@
         <v>32</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>287</v>
+        <v>322</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="E109" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>3</v>
+        <v>312</v>
       </c>
       <c r="G109" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H109" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I109" s="32"/>
     </row>
-    <row r="110" spans="1:9" ht="30">
+    <row r="110" spans="1:9" ht="75">
       <c r="A110" s="30" t="s">
         <v>132</v>
       </c>
@@ -5119,26 +5158,24 @@
         <v>32</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>288</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>321</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="D110" s="30"/>
       <c r="E110" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F110" s="30" t="s">
-        <v>329</v>
+        <v>3</v>
       </c>
       <c r="G110" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H110" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9" ht="75">
+    <row r="111" spans="1:9">
       <c r="A111" s="30" t="s">
         <v>133</v>
       </c>
@@ -5146,24 +5183,24 @@
         <v>32</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="D111" s="30"/>
       <c r="E111" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F111" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G111" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H111" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9">
+    <row r="112" spans="1:9" ht="30">
       <c r="A112" s="30" t="s">
         <v>134</v>
       </c>
@@ -5171,64 +5208,64 @@
         <v>32</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F112" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G112" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H112" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="30">
+    <row r="113" spans="1:9">
       <c r="A113" s="30" t="s">
         <v>135</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>32</v>
+        <v>187</v>
       </c>
       <c r="C113" s="32" t="s">
-        <v>291</v>
+        <v>244</v>
       </c>
       <c r="D113" s="30"/>
       <c r="E113" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F113" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G113" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H113" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9">
+    <row r="114" spans="1:9" ht="30">
       <c r="A114" s="30" t="s">
         <v>136</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>248</v>
+        <v>281</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F114" s="30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="G114" s="30" t="s">
         <v>16</v>
@@ -5243,10 +5280,10 @@
         <v>137</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="D115" s="30"/>
       <c r="E115" s="30" t="s">
@@ -5256,22 +5293,22 @@
         <v>7</v>
       </c>
       <c r="G115" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H115" s="30" t="s">
         <v>18</v>
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" ht="45">
+    <row r="116" spans="1:9">
       <c r="A116" s="30" t="s">
         <v>138</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30" t="s">
@@ -5293,35 +5330,35 @@
         <v>139</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F117" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G117" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H117" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" ht="30">
+    <row r="118" spans="1:9">
       <c r="A118" s="30" t="s">
         <v>140</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30" t="s">
@@ -5338,15 +5375,15 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9" ht="45">
+    <row r="119" spans="1:9">
       <c r="A119" s="30" t="s">
         <v>141</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C119" s="32" t="s">
-        <v>296</v>
+        <v>250</v>
       </c>
       <c r="D119" s="30"/>
       <c r="E119" s="30" t="s">
@@ -5363,7 +5400,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9">
       <c r="A120" s="30" t="s">
         <v>142</v>
       </c>
@@ -5371,42 +5408,42 @@
         <v>191</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F120" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G120" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H120" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:9" ht="60">
       <c r="A121" s="30" t="s">
         <v>143</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>255</v>
+        <v>287</v>
       </c>
       <c r="D121" s="30"/>
       <c r="E121" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F121" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G121" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H121" s="30" t="s">
         <v>18</v>
@@ -5418,17 +5455,17 @@
         <v>144</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F122" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G122" s="30" t="s">
         <v>16</v>
@@ -5438,40 +5475,40 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="60">
+    <row r="123" spans="1:9" ht="120">
       <c r="A123" s="30" t="s">
         <v>145</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="D123" s="30"/>
       <c r="E123" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F123" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G123" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H123" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" ht="30">
+    <row r="124" spans="1:9">
       <c r="A124" s="30" t="s">
         <v>146</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30" t="s">
@@ -5481,22 +5518,22 @@
         <v>6</v>
       </c>
       <c r="G124" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H124" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" ht="120">
+    <row r="125" spans="1:9">
       <c r="A125" s="30" t="s">
         <v>147</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C125" s="32" t="s">
-        <v>301</v>
+        <v>266</v>
       </c>
       <c r="D125" s="30"/>
       <c r="E125" s="30" t="s">
@@ -5506,10 +5543,10 @@
         <v>6</v>
       </c>
       <c r="G125" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H125" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I125" s="32"/>
     </row>
@@ -5520,8 +5557,8 @@
       <c r="B126" s="31" t="s">
         <v>194</v>
       </c>
-      <c r="C126" s="32" t="s">
-        <v>302</v>
+      <c r="C126" s="20" t="s">
+        <v>324</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30" t="s">
@@ -5531,22 +5568,22 @@
         <v>6</v>
       </c>
       <c r="G126" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H126" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="30">
+    <row r="127" spans="1:9" ht="135">
       <c r="A127" s="30" t="s">
         <v>149</v>
       </c>
       <c r="B127" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>272</v>
+        <v>291</v>
       </c>
       <c r="D127" s="30"/>
       <c r="E127" s="30" t="s">
@@ -5556,10 +5593,10 @@
         <v>6</v>
       </c>
       <c r="G127" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H127" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I127" s="32"/>
     </row>
@@ -5568,10 +5605,10 @@
         <v>150</v>
       </c>
       <c r="B128" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
       <c r="D128" s="30"/>
       <c r="E128" s="30" t="s">
@@ -5581,22 +5618,22 @@
         <v>6</v>
       </c>
       <c r="G128" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H128" s="30" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="135">
-      <c r="A129" s="30" t="s">
+    <row r="129" spans="1:9" ht="45">
+      <c r="A129" s="22" t="s">
         <v>151</v>
       </c>
       <c r="B129" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="C129" s="32" t="s">
-        <v>304</v>
+        <v>194</v>
+      </c>
+      <c r="C129" s="20" t="s">
+        <v>325</v>
       </c>
       <c r="D129" s="30"/>
       <c r="E129" s="30" t="s">
@@ -5609,19 +5646,21 @@
         <v>15</v>
       </c>
       <c r="H129" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I129" s="32"/>
-    </row>
-    <row r="130" spans="1:9" ht="30">
+        <v>17</v>
+      </c>
+      <c r="I129" s="20" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9">
       <c r="A130" s="30" t="s">
         <v>152</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="C130" s="32" t="s">
-        <v>305</v>
+        <v>194</v>
+      </c>
+      <c r="C130" s="20" t="s">
+        <v>326</v>
       </c>
       <c r="D130" s="30"/>
       <c r="E130" s="30" t="s">
@@ -5634,19 +5673,19 @@
         <v>15</v>
       </c>
       <c r="H130" s="30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="45">
+    <row r="131" spans="1:9" ht="30">
       <c r="A131" s="30" t="s">
         <v>153</v>
       </c>
       <c r="B131" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="D131" s="30"/>
       <c r="E131" s="30" t="s">
@@ -5659,21 +5698,19 @@
         <v>15</v>
       </c>
       <c r="H131" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I131" s="32" t="s">
-        <v>330</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I131" s="32"/>
     </row>
     <row r="132" spans="1:9" ht="30">
       <c r="A132" s="30" t="s">
         <v>154</v>
       </c>
       <c r="B132" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D132" s="30"/>
       <c r="E132" s="30" t="s">
@@ -5695,10 +5732,10 @@
         <v>155</v>
       </c>
       <c r="B133" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="C133" s="32" t="s">
-        <v>308</v>
+        <v>194</v>
+      </c>
+      <c r="C133" s="20" t="s">
+        <v>327</v>
       </c>
       <c r="D133" s="30"/>
       <c r="E133" s="30" t="s">
@@ -5720,17 +5757,17 @@
         <v>156</v>
       </c>
       <c r="B134" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="D134" s="30"/>
       <c r="E134" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F134" s="30" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G134" s="30" t="s">
         <v>15</v>
@@ -5740,174 +5777,182 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="30">
+    <row r="135" spans="1:9" ht="45">
       <c r="A135" s="30" t="s">
         <v>157</v>
       </c>
       <c r="B135" s="31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="D135" s="30"/>
       <c r="E135" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F135" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G135" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H135" s="30" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I135" s="32"/>
     </row>
-    <row r="136" spans="1:9" ht="30">
+    <row r="136" spans="1:9" ht="45">
       <c r="A136" s="30" t="s">
         <v>158</v>
       </c>
       <c r="B136" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>311</v>
-      </c>
-      <c r="D136" s="30"/>
+        <v>297</v>
+      </c>
+      <c r="D136" s="30" t="s">
+        <v>305</v>
+      </c>
       <c r="E136" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F136" s="30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G136" s="30" t="s">
         <v>15</v>
       </c>
       <c r="H136" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I136" s="32"/>
+        <v>21</v>
+      </c>
+      <c r="I136" s="32" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="137" spans="1:9" ht="45">
       <c r="A137" s="30" t="s">
         <v>159</v>
       </c>
       <c r="B137" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C137" s="32" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="D137" s="30"/>
       <c r="E137" s="30" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F137" s="30" t="s">
         <v>3</v>
       </c>
       <c r="G137" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H137" s="30" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="45">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="30" t="s">
         <v>160</v>
       </c>
       <c r="B138" s="31" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C138" s="32" t="s">
-        <v>313</v>
-      </c>
-      <c r="D138" s="30" t="s">
-        <v>322</v>
-      </c>
+        <v>299</v>
+      </c>
+      <c r="D138" s="30"/>
       <c r="E138" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F138" s="30" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G138" s="30" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H138" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="I138" s="32" t="s">
-        <v>330</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I138" s="32"/>
     </row>
     <row r="139" spans="1:9" ht="45">
       <c r="A139" s="30" t="s">
         <v>161</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C139" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="D139" s="30"/>
+        <v>195</v>
+      </c>
+      <c r="C139" s="20" t="s">
+        <v>328</v>
+      </c>
+      <c r="D139" s="30" t="s">
+        <v>306</v>
+      </c>
       <c r="E139" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F139" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G139" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H139" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I139" s="32"/>
-    </row>
-    <row r="140" spans="1:9" ht="30">
-      <c r="A140" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I139" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="45">
+      <c r="A140" s="22" t="s">
         <v>162</v>
       </c>
       <c r="B140" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C140" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="D140" s="30"/>
+        <v>195</v>
+      </c>
+      <c r="C140" s="20" t="s">
+        <v>314</v>
+      </c>
+      <c r="D140" s="30" t="s">
+        <v>306</v>
+      </c>
       <c r="E140" s="30" t="s">
         <v>22</v>
       </c>
       <c r="F140" s="30" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G140" s="30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H140" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I140" s="32"/>
+        <v>20</v>
+      </c>
+      <c r="I140" s="32" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="141" spans="1:9" ht="45">
-      <c r="A141" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="B141" s="31" t="s">
-        <v>197</v>
+      <c r="A141" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="B141" s="24" t="s">
+        <v>195</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>331</v>
-      </c>
-      <c r="D141" s="30" t="s">
-        <v>323</v>
-      </c>
-      <c r="E141" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="D141" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="E141" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F141" s="30" t="s">
@@ -5920,23 +5965,23 @@
         <v>20</v>
       </c>
       <c r="I141" s="32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" ht="45">
-      <c r="A142" s="30" t="s">
-        <v>164</v>
-      </c>
-      <c r="B142" s="31" t="s">
-        <v>197</v>
+        <v>309</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" ht="60">
+      <c r="A142" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="B142" s="24" t="s">
+        <v>195</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>332</v>
-      </c>
-      <c r="D142" s="30" t="s">
-        <v>323</v>
-      </c>
-      <c r="E142" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="D142" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="E142" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F142" s="30" t="s">
@@ -5949,21 +5994,23 @@
         <v>20</v>
       </c>
       <c r="I142" s="32" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="30">
-      <c r="A143" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="B143" s="31" t="s">
-        <v>197</v>
-      </c>
-      <c r="C143" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="D143" s="30"/>
-      <c r="E143" s="30" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="45">
+      <c r="A143" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="B143" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C143" s="20" t="s">
+        <v>337</v>
+      </c>
+      <c r="D143" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="E143" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F143" s="30" t="s">
@@ -5973,20 +6020,81 @@
         <v>15</v>
       </c>
       <c r="H143" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I143" s="32"/>
-    </row>
-    <row r="144" spans="1:9">
-      <c r="A144" s="3"/>
-      <c r="B144" s="10"/>
-    </row>
-    <row r="145" spans="1:2">
-      <c r="A145" s="3"/>
-      <c r="B145" s="10"/>
+        <v>20</v>
+      </c>
+      <c r="I143" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="45">
+      <c r="A144" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B144" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C144" s="20" t="s">
+        <v>338</v>
+      </c>
+      <c r="D144" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="E144" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F144" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G144" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H144" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I144" s="32" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" ht="45">
+      <c r="A145" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B145" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C145" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="D145" s="30"/>
+      <c r="E145" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F145" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G145" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H145" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I145" s="32"/>
+    </row>
+    <row r="146" spans="1:9">
+      <c r="A146" s="3"/>
+      <c r="B146" s="10"/>
+    </row>
+    <row r="147" spans="1:9">
+      <c r="A147" s="3"/>
+      <c r="B147" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -5994,80 +6102,53 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H143 A34:I143">
-    <cfRule type="expression" dxfId="32" priority="53">
+  <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
+    <cfRule type="expression" dxfId="26" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="54">
+    <cfRule type="expression" dxfId="25" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="61">
+    <cfRule type="expression" dxfId="24" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H143 A34:I143">
-    <cfRule type="expression" dxfId="29" priority="7">
+  <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
+    <cfRule type="expression" dxfId="23" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="8">
+    <cfRule type="expression" dxfId="22" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="9">
+    <cfRule type="expression" dxfId="21" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F143">
-    <cfRule type="expression" dxfId="26" priority="13">
+  <conditionalFormatting sqref="F20:F145">
+    <cfRule type="expression" dxfId="20" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I143">
-    <cfRule type="expression" dxfId="24" priority="4">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="23" priority="5">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="6">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I20:I143">
-    <cfRule type="expression" dxfId="21" priority="1">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2">
-      <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="3">
-      <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F143">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F145">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E143">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E145">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G143">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G145">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H143">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H145">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6077,7 +6158,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B19:B145 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B144:B147 B19:B143 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -6093,15 +6174,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -6150,6 +6222,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
@@ -6165,14 +6246,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6185,4 +6258,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
[MS-AUTHWS] Update capture code for fixed bugs
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-AUTHWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Interop_TestSuites\SharePoint\Docs\MS-AUTHWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="343">
   <si>
     <t>Req ID</t>
   </si>
@@ -1333,20 +1333,24 @@
   <si>
     <t>[In Appendix B: Product Behavior] &lt;4&gt; Section 3.1.4.2.4.1: Use of Windows Live ID for authentication is not supported by Windows Server 2008 operating system with Service Pack 2 (SP2) and Windows Server 2012 operating system.</t>
   </si>
+  <si>
+    <t>Unverified</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1548,13 +1552,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1587,7 +1591,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1612,6 +1616,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1635,21 +1654,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2592,127 +2596,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -2725,12 +2729,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -2743,12 +2747,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -2761,12 +2765,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -2779,60 +2783,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -3272,7 +3276,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" ht="30">
+    <row r="36" spans="1:9">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -3347,7 +3351,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30">
+    <row r="39" spans="1:9">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
@@ -3597,7 +3601,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" ht="30">
+    <row r="49" spans="1:9">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
@@ -3672,7 +3676,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="45">
+    <row r="52" spans="1:9" ht="30">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
@@ -3897,7 +3901,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30">
+    <row r="61" spans="1:9">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
@@ -4628,7 +4632,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="30">
+    <row r="90" spans="1:9">
       <c r="A90" s="30" t="s">
         <v>112</v>
       </c>
@@ -5939,7 +5943,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="45">
+    <row r="141" spans="1:9" ht="30">
       <c r="A141" s="22" t="s">
         <v>329</v>
       </c>
@@ -5962,11 +5966,9 @@
         <v>15</v>
       </c>
       <c r="H141" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I141" s="32" t="s">
-        <v>309</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I141" s="32"/>
     </row>
     <row r="142" spans="1:9" ht="60">
       <c r="A142" s="22" t="s">
@@ -6019,12 +6021,10 @@
       <c r="G143" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H143" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I143" s="32" t="s">
-        <v>309</v>
-      </c>
+      <c r="H143" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="I143" s="32"/>
     </row>
     <row r="144" spans="1:9" ht="45">
       <c r="A144" s="22" t="s">
@@ -6090,11 +6090,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -6102,6 +6097,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
@@ -6168,12 +6168,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -6222,6 +6216,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -6232,20 +6232,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6260,6 +6246,20 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
[MS-AUTHWS]: Fix watchman warnings.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Interop_TestSuites\SharePoint\Docs\MS-AUTHWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Github\Interop-TestSuites2\SharePoint\Docs\MS-AUTHWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="343">
   <si>
     <t>Req ID</t>
   </si>
@@ -1325,17 +1325,17 @@
     <t>[In Appendix B: Product Behavior] Implementation does not use authentication if the AuthenticationMode is "None". (Windows SharePoint Services 3.0, Microsoft SharePoint Foundation 2013 and Microsoft SharePoint Server 2016 follow this behavior.)</t>
   </si>
   <si>
-    <t>Verified by derived requirements: MS-AUTHWS_R190,MS-AUTHWS_R191.</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-AUTHWS_R192,MS-AUTHWS_R193.</t>
-  </si>
-  <si>
     <t>[In Appendix B: Product Behavior] &lt;4&gt; Section 3.1.4.2.4.1: Use of Windows Live ID for authentication is not supported by Windows Server 2008 operating system with Service Pack 2 (SP2) and Windows Server 2012 operating system.</t>
   </si>
   <si>
     <t>Unverified</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-AUTHWS_R191.</t>
+  </si>
+  <si>
+    <t>Verified by derived requirement: MS-AUTHWS_R193.</t>
   </si>
 </sst>
 </file>
@@ -1343,14 +1343,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1552,13 +1552,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1591,7 +1591,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3276,7 +3276,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -3351,7 +3351,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9">
+    <row r="39" spans="1:9" ht="30">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
@@ -3601,7 +3601,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" ht="30">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="30">
+    <row r="52" spans="1:9" ht="45">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
@@ -3901,14 +3901,14 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
       <c r="B61" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="32" t="s">
+      <c r="C61" s="20" t="s">
         <v>317</v>
       </c>
       <c r="D61" s="30"/>
@@ -4632,7 +4632,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="90" spans="1:9">
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="30" t="s">
         <v>112</v>
       </c>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="45">
+    <row r="92" spans="1:9" ht="30">
       <c r="A92" s="22" t="s">
         <v>114</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>17</v>
       </c>
       <c r="I92" s="20" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
     </row>
     <row r="93" spans="1:9">
@@ -4913,7 +4913,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="45">
+    <row r="101" spans="1:9" ht="30">
       <c r="A101" s="30" t="s">
         <v>123</v>
       </c>
@@ -4938,9 +4938,7 @@
       <c r="H101" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I101" s="20" t="s">
-        <v>313</v>
-      </c>
+      <c r="I101" s="20"/>
     </row>
     <row r="102" spans="1:9" ht="45">
       <c r="A102" s="30" t="s">
@@ -5053,7 +5051,7 @@
       <c r="B106" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C106" s="32" t="s">
+      <c r="C106" s="20" t="s">
         <v>319</v>
       </c>
       <c r="D106" s="30" t="s">
@@ -5080,7 +5078,7 @@
       <c r="B107" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C107" s="32" t="s">
+      <c r="C107" s="20" t="s">
         <v>320</v>
       </c>
       <c r="D107" s="30" t="s">
@@ -5107,7 +5105,7 @@
       <c r="B108" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="C108" s="32" t="s">
+      <c r="C108" s="20" t="s">
         <v>321</v>
       </c>
       <c r="D108" s="30" t="s">
@@ -5580,7 +5578,7 @@
       <c r="I126" s="32"/>
     </row>
     <row r="127" spans="1:9" ht="135">
-      <c r="A127" s="30" t="s">
+      <c r="A127" s="22" t="s">
         <v>149</v>
       </c>
       <c r="B127" s="31" t="s">
@@ -5629,7 +5627,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="45">
+    <row r="129" spans="1:9" ht="30">
       <c r="A129" s="22" t="s">
         <v>151</v>
       </c>
@@ -5653,7 +5651,7 @@
         <v>17</v>
       </c>
       <c r="I129" s="20" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="130" spans="1:9">
@@ -6022,7 +6020,7 @@
         <v>15</v>
       </c>
       <c r="H143" s="22" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="I143" s="32"/>
     </row>
@@ -6063,7 +6061,7 @@
         <v>195</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D145" s="30"/>
       <c r="E145" s="30" t="s">
@@ -6168,6 +6166,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F2EA47BB262D974097182E2CA8AB13E1" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="74597e8d9e42e7e4fc8eda6d37675aa2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aeb20c0e3442673af7ee10786458764">
     <xsd:element name="properties">
@@ -6216,22 +6223,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EDB2DE12-5EF6-4CF2-820D-5F9FE329E08E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6246,7 +6252,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6258,12 +6264,4 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
MS-MEETS: Update RS according to v20190618 document. Update capture code in test suite and add SharePoint 2019 ptfconfig file.
MS-AUTHWS:
Update RS according to v20190618 document.

MS-DWSS:
Update RS according to v20190618 document.
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanff\Source\Repos\MAPITEST-Interop-TestSuites\SharePoint\Docs\MS-AUTHWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF23B38-04C4-4C83-9D6E-883DA0692808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDB75A8-5925-44E3-9827-95F16E5D2265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1195,9 +1195,6 @@
     <t>[In Appendix B: Product Behavior] Implementation does additionally support SOAP over HTTPS to help secure communication with protocol clients.(The Windows SharePoint Services 3.0 and above products follow this behavior.)</t>
   </si>
   <si>
-    <t>[In Appendix B: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms SHOULD or SHOULD NOT implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
-  </si>
-  <si>
     <t>MS-AUTHWS_R3:c</t>
   </si>
   <si>
@@ -1339,6 +1336,10 @@
   </si>
   <si>
     <t>[In Appendix B: Product Behavior] Unless otherwise specified, the term "MAY" implies that the product does not follow the prescription.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms "SHOULD" or "SHOULD NOT" implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1400,6 +1401,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1620,6 +1622,21 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1643,21 +1660,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2546,8 +2548,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:I6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,7 +2569,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2577,7 +2579,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2594,7 +2596,7 @@
         <v>4</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F3" s="12">
         <v>43634</v>
@@ -2602,127 +2604,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
-      <c r="G5" s="46"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="46"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="36"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="43" t="s">
+      <c r="B7" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
+      <c r="C9" s="44"/>
+      <c r="D9" s="44"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="39"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="39"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2735,12 +2737,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2753,12 +2755,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36"/>
-      <c r="F13" s="36"/>
-      <c r="G13" s="36"/>
-      <c r="H13" s="36"/>
-      <c r="I13" s="36"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2771,12 +2773,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36"/>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2789,60 +2791,60 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37"/>
-      <c r="F15" s="37"/>
-      <c r="G15" s="37"/>
-      <c r="H15" s="37"/>
-      <c r="I15" s="37"/>
+      <c r="D15" s="42"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="39"/>
+      <c r="F16" s="39"/>
+      <c r="G16" s="39"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="40" t="s">
+      <c r="B17" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="41"/>
+      <c r="C17" s="46"/>
+      <c r="D17" s="46"/>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="39"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -2925,7 +2927,7 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
@@ -2964,7 +2966,7 @@
         <v>199</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>19</v>
@@ -2991,7 +2993,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>19</v>
@@ -3315,7 +3317,7 @@
         <v>166</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30" t="s">
@@ -3340,7 +3342,7 @@
         <v>166</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30" t="s">
@@ -3722,7 +3724,7 @@
         <v>19</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>15</v>
@@ -3890,7 +3892,7 @@
         <v>176</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -3915,7 +3917,7 @@
         <v>31</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
@@ -3993,7 +3995,7 @@
         <v>236</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>19</v>
@@ -4020,7 +4022,7 @@
         <v>237</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E65" s="30" t="s">
         <v>19</v>
@@ -4136,7 +4138,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="30" t="s">
         <v>92</v>
       </c>
@@ -4211,7 +4213,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="30" t="s">
         <v>95</v>
       </c>
@@ -4261,7 +4263,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A75" s="30" t="s">
         <v>97</v>
       </c>
@@ -4286,7 +4288,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="30" t="s">
         <v>98</v>
       </c>
@@ -4311,7 +4313,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="30" t="s">
         <v>99</v>
       </c>
@@ -4361,7 +4363,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A79" s="30" t="s">
         <v>101</v>
       </c>
@@ -4386,7 +4388,7 @@
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A80" s="30" t="s">
         <v>102</v>
       </c>
@@ -4411,7 +4413,7 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="30" t="s">
         <v>103</v>
       </c>
@@ -4461,7 +4463,7 @@
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="30" t="s">
         <v>105</v>
       </c>
@@ -4486,7 +4488,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A84" s="30" t="s">
         <v>106</v>
       </c>
@@ -4511,7 +4513,7 @@
       </c>
       <c r="I84" s="32"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="30" t="s">
         <v>107</v>
       </c>
@@ -4536,7 +4538,7 @@
       </c>
       <c r="I85" s="32"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="30" t="s">
         <v>108</v>
       </c>
@@ -4635,7 +4637,7 @@
         <v>17</v>
       </c>
       <c r="I89" s="20" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -4663,7 +4665,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A91" s="30" t="s">
         <v>113</v>
       </c>
@@ -4696,7 +4698,7 @@
         <v>184</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30" t="s">
@@ -4712,10 +4714,10 @@
         <v>17</v>
       </c>
       <c r="I92" s="20" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A93" s="30" t="s">
         <v>115</v>
       </c>
@@ -4740,7 +4742,7 @@
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A94" s="30" t="s">
         <v>116</v>
       </c>
@@ -4876,7 +4878,7 @@
         <v>270</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E99" s="30" t="s">
         <v>19</v>
@@ -4903,7 +4905,7 @@
         <v>271</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>19</v>
@@ -4930,7 +4932,7 @@
         <v>272</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E101" s="30" t="s">
         <v>19</v>
@@ -4982,7 +4984,7 @@
         <v>274</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E103" s="30" t="s">
         <v>19</v>
@@ -5009,7 +5011,7 @@
         <v>275</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E104" s="30" t="s">
         <v>19</v>
@@ -5033,7 +5035,7 @@
         <v>32</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D105" s="30"/>
       <c r="E105" s="30" t="s">
@@ -5058,10 +5060,10 @@
         <v>32</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E106" s="30" t="s">
         <v>19</v>
@@ -5085,10 +5087,10 @@
         <v>32</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E107" s="30" t="s">
         <v>19</v>
@@ -5112,10 +5114,10 @@
         <v>32</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E108" s="30" t="s">
         <v>19</v>
@@ -5139,16 +5141,16 @@
         <v>32</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E109" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G109" s="30" t="s">
         <v>15</v>
@@ -5233,7 +5235,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A113" s="30" t="s">
         <v>135</v>
       </c>
@@ -5308,7 +5310,7 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="30" t="s">
         <v>138</v>
       </c>
@@ -5358,7 +5360,7 @@
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A118" s="30" t="s">
         <v>140</v>
       </c>
@@ -5383,7 +5385,7 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A119" s="30" t="s">
         <v>141</v>
       </c>
@@ -5408,7 +5410,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="30" t="s">
         <v>142</v>
       </c>
@@ -5458,7 +5460,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="30" t="s">
         <v>144</v>
       </c>
@@ -5508,7 +5510,7 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A124" s="30" t="s">
         <v>146</v>
       </c>
@@ -5533,7 +5535,7 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="30" t="s">
         <v>147</v>
       </c>
@@ -5566,7 +5568,7 @@
         <v>194</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30" t="s">
@@ -5641,7 +5643,7 @@
         <v>194</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D129" s="30"/>
       <c r="E129" s="30" t="s">
@@ -5657,10 +5659,10 @@
         <v>17</v>
       </c>
       <c r="I129" s="20" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="30" t="s">
         <v>152</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>194</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D130" s="30"/>
       <c r="E130" s="30" t="s">
@@ -5743,7 +5745,7 @@
         <v>194</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D133" s="30"/>
       <c r="E133" s="30" t="s">
@@ -5821,7 +5823,7 @@
         <v>295</v>
       </c>
       <c r="D136" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E136" s="30" t="s">
         <v>22</v>
@@ -5836,7 +5838,7 @@
         <v>21</v>
       </c>
       <c r="I136" s="32" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="137" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5846,8 +5848,8 @@
       <c r="B137" s="31" t="s">
         <v>195</v>
       </c>
-      <c r="C137" s="32" t="s">
-        <v>296</v>
+      <c r="C137" s="20" t="s">
+        <v>342</v>
       </c>
       <c r="D137" s="30"/>
       <c r="E137" s="30" t="s">
@@ -5872,7 +5874,7 @@
         <v>195</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D138" s="30"/>
       <c r="E138" s="30" t="s">
@@ -5897,10 +5899,10 @@
         <v>195</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D139" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E139" s="30" t="s">
         <v>22</v>
@@ -5915,7 +5917,7 @@
         <v>20</v>
       </c>
       <c r="I139" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -5926,10 +5928,10 @@
         <v>195</v>
       </c>
       <c r="C140" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D140" s="30" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E140" s="30" t="s">
         <v>22</v>
@@ -5944,21 +5946,21 @@
         <v>20</v>
       </c>
       <c r="I140" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B141" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E141" s="33" t="s">
         <v>22</v>
@@ -5976,16 +5978,16 @@
     </row>
     <row r="142" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A142" s="22" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B142" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E142" s="33" t="s">
         <v>22</v>
@@ -6000,21 +6002,21 @@
         <v>20</v>
       </c>
       <c r="I142" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A143" s="22" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B143" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E143" s="33" t="s">
         <v>22</v>
@@ -6026,22 +6028,22 @@
         <v>15</v>
       </c>
       <c r="H143" s="22" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I143" s="32"/>
     </row>
     <row r="144" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A144" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E144" s="33" t="s">
         <v>22</v>
@@ -6056,7 +6058,7 @@
         <v>20</v>
       </c>
       <c r="I144" s="32" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -6067,7 +6069,7 @@
         <v>195</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D145" s="30"/>
       <c r="E145" s="30" t="s">
@@ -6094,11 +6096,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -6106,6 +6103,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
@@ -6221,18 +6223,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6251,14 +6253,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -6270,4 +6264,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B6D33261-F3C6-4621-88F1-D76E5ABE1865}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated RS, md file, configuraton files and code for MS-AUTHWS(20220215).
</commit_message>
<xml_diff>
--- a/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
+++ b/SharePoint/Docs/MS-AUTHWS/MS-AUTHWS_RequirementSpecification.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fanff\Source\Repos\MAPITEST-Interop-TestSuites\SharePoint\Docs\MS-AUTHWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\v-jingym\source\repos\Interop-TestSuites\SharePoint\Docs\MS-AUTHWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FDB75A8-5925-44E3-9827-95F16E5D2265}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64EB8C21-C5C3-479A-B821-C112FDA19FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$145</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$146</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="967" uniqueCount="346">
   <si>
     <t>Req ID</t>
   </si>
@@ -1103,9 +1103,6 @@
     <t>[In LoginErrorCode] The value of LoginErrorCode is "NotInFormsAuthenticationMode", when the Login operation failed because the authentication mode is set to Passport authentication.</t>
   </si>
   <si>
-    <t>[In LoginErrorCode] The value of LoginErrorCode is "PasswordNotMatch", when the Login operation failed because the logon name is not found by the server, or the password does not match what is stored on the server.</t>
-  </si>
-  <si>
     <t>[In LoginErrorCode] The value of LoginErrorCode is "PasswordNotMatch", when the Login operation failed because the logon name is not found by the server, [or the password does not match what is stored on the server].</t>
   </si>
   <si>
@@ -1342,20 +1339,32 @@
     <t>[In Appendix B: Product Behavior] Unless otherwise specified, any statement of optional behavior in this specification that is prescribed using the terms "SHOULD" or "SHOULD NOT" implies product behavior in accordance with the SHOULD or SHOULD NOT prescription.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>MS-AUTHWS_R830</t>
+  </si>
+  <si>
+    <t>[In Appendix B: Product Behavior] A SOAP exception is returned when the Login operation failed because the logon name is not found by the server, or the password does not match what is stored on the server. (&lt;3&gt; Section 3.1.4.21.4.1:  SharePoint Server Subscription Edition returns a SOAP exception.)</t>
+  </si>
+  <si>
+    <t>MS-AUTHWS_R83:i</t>
+  </si>
+  <si>
+    <t>[In LoginErrorCode] The value of LoginErrorCode is "PasswordNotMatch", when the Login operation failed because the logon name is not found by the server, or the password does not match what is stored on the server .&lt;3&gt;  (Microsoft SharePoint 2007，2010,  2013, 2016 and  2019 follow this behavior)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="0.0.0"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="0.0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1402,6 +1411,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1549,7 +1563,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1558,13 +1572,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1597,7 +1611,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1620,6 +1634,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1663,9 +1680,53 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="27">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2004,50 +2065,6 @@
         <scheme val="none"/>
       </font>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2177,34 +2194,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I145" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I145" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I146" tableType="xml" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25" connectionId="1">
+  <autoFilter ref="A19:I146" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="24">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="23">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -2213,19 +2230,19 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2546,30 +2563,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L147"/>
+  <dimension ref="A1:L148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C137" sqref="C137"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16" style="11" customWidth="1"/>
-    <col min="2" max="2" width="6.875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
     <col min="10" max="11" width="9" style="3" customWidth="1"/>
     <col min="12" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>26</v>
@@ -2577,9 +2594,9 @@
       <c r="F1" s="4"/>
       <c r="J1" s="5"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" s="6" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
@@ -2588,146 +2605,146 @@
       <c r="F2" s="25"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C3" s="29">
-        <v>4</v>
+        <v>8.1</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="F3" s="12">
-        <v>43634</v>
+        <v>44607</v>
       </c>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="34" t="s">
+    <row r="4" spans="1:10" ht="21">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="H8" s="35"/>
-      <c r="I8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
-      <c r="F10" s="44"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12" s="26" t="s">
         <v>8</v>
       </c>
@@ -2737,15 +2754,15 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="15" customHeight="1">
       <c r="A13" s="27" t="s">
         <v>6</v>
       </c>
@@ -2755,15 +2772,15 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14" s="27" t="s">
         <v>7</v>
       </c>
@@ -2773,15 +2790,15 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="41"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15" s="28" t="s">
         <v>3</v>
       </c>
@@ -2791,64 +2808,64 @@
       <c r="C15" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="39" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:12" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="46"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="39" t="s">
+      <c r="B18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
-    <row r="19" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" ht="30">
       <c r="A19" s="3" t="s">
         <v>0</v>
       </c>
@@ -2878,7 +2895,7 @@
       </c>
       <c r="J19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:12" s="23" customFormat="1">
       <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
@@ -2903,7 +2920,7 @@
       </c>
       <c r="I20" s="24"/>
     </row>
-    <row r="21" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A21" s="22" t="s">
         <v>43</v>
       </c>
@@ -2927,10 +2944,10 @@
         <v>17</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A22" s="22" t="s">
         <v>44</v>
       </c>
@@ -2955,7 +2972,7 @@
       </c>
       <c r="I22" s="24"/>
     </row>
-    <row r="23" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A23" s="22" t="s">
         <v>45</v>
       </c>
@@ -2966,7 +2983,7 @@
         <v>199</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E23" s="22" t="s">
         <v>19</v>
@@ -2982,7 +2999,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:12" s="23" customFormat="1">
       <c r="A24" s="22" t="s">
         <v>46</v>
       </c>
@@ -2993,7 +3010,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E24" s="22" t="s">
         <v>19</v>
@@ -3009,7 +3026,7 @@
       </c>
       <c r="I24" s="24"/>
     </row>
-    <row r="25" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A25" s="22" t="s">
         <v>47</v>
       </c>
@@ -3034,7 +3051,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A26" s="22" t="s">
         <v>48</v>
       </c>
@@ -3059,7 +3076,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A27" s="22" t="s">
         <v>49</v>
       </c>
@@ -3084,7 +3101,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A28" s="22" t="s">
         <v>50</v>
       </c>
@@ -3109,7 +3126,7 @@
       </c>
       <c r="I28" s="24"/>
     </row>
-    <row r="29" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A29" s="22" t="s">
         <v>51</v>
       </c>
@@ -3134,7 +3151,7 @@
       </c>
       <c r="I29" s="24"/>
     </row>
-    <row r="30" spans="1:12" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
@@ -3159,7 +3176,7 @@
       </c>
       <c r="I30" s="24"/>
     </row>
-    <row r="31" spans="1:12" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A31" s="22" t="s">
         <v>53</v>
       </c>
@@ -3184,7 +3201,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A32" s="22" t="s">
         <v>54</v>
       </c>
@@ -3209,7 +3226,7 @@
       </c>
       <c r="I32" s="24"/>
     </row>
-    <row r="33" spans="1:9" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:9" s="23" customFormat="1" ht="30">
       <c r="A33" s="22" t="s">
         <v>55</v>
       </c>
@@ -3234,7 +3251,7 @@
       </c>
       <c r="I33" s="24"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="30">
       <c r="A34" s="30" t="s">
         <v>56</v>
       </c>
@@ -3259,7 +3276,7 @@
       </c>
       <c r="I34" s="32"/>
     </row>
-    <row r="35" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="30">
       <c r="A35" s="30" t="s">
         <v>57</v>
       </c>
@@ -3284,7 +3301,7 @@
       </c>
       <c r="I35" s="32"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="30" t="s">
         <v>58</v>
       </c>
@@ -3309,7 +3326,7 @@
       </c>
       <c r="I36" s="32"/>
     </row>
-    <row r="37" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="45">
       <c r="A37" s="30" t="s">
         <v>59</v>
       </c>
@@ -3317,7 +3334,7 @@
         <v>166</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D37" s="30"/>
       <c r="E37" s="30" t="s">
@@ -3334,7 +3351,7 @@
       </c>
       <c r="I37" s="32"/>
     </row>
-    <row r="38" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="45">
       <c r="A38" s="30" t="s">
         <v>60</v>
       </c>
@@ -3342,7 +3359,7 @@
         <v>166</v>
       </c>
       <c r="C38" s="20" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D38" s="30"/>
       <c r="E38" s="30" t="s">
@@ -3359,7 +3376,7 @@
       </c>
       <c r="I38" s="32"/>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="30">
       <c r="A39" s="30" t="s">
         <v>61</v>
       </c>
@@ -3384,7 +3401,7 @@
       </c>
       <c r="I39" s="32"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="30">
       <c r="A40" s="30" t="s">
         <v>62</v>
       </c>
@@ -3409,7 +3426,7 @@
       </c>
       <c r="I40" s="32"/>
     </row>
-    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30">
       <c r="A41" s="30" t="s">
         <v>63</v>
       </c>
@@ -3434,7 +3451,7 @@
       </c>
       <c r="I41" s="32"/>
     </row>
-    <row r="42" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="30">
       <c r="A42" s="30" t="s">
         <v>64</v>
       </c>
@@ -3459,7 +3476,7 @@
       </c>
       <c r="I42" s="32"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30">
       <c r="A43" s="30" t="s">
         <v>65</v>
       </c>
@@ -3484,7 +3501,7 @@
       </c>
       <c r="I43" s="32"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="30">
       <c r="A44" s="30" t="s">
         <v>66</v>
       </c>
@@ -3509,7 +3526,7 @@
       </c>
       <c r="I44" s="32"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="30">
       <c r="A45" s="30" t="s">
         <v>67</v>
       </c>
@@ -3534,7 +3551,7 @@
       </c>
       <c r="I45" s="32"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="30">
       <c r="A46" s="30" t="s">
         <v>68</v>
       </c>
@@ -3559,7 +3576,7 @@
       </c>
       <c r="I46" s="32"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="30">
       <c r="A47" s="30" t="s">
         <v>69</v>
       </c>
@@ -3584,7 +3601,7 @@
       </c>
       <c r="I47" s="32"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9">
       <c r="A48" s="30" t="s">
         <v>70</v>
       </c>
@@ -3609,7 +3626,7 @@
       </c>
       <c r="I48" s="32"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="30">
       <c r="A49" s="30" t="s">
         <v>71</v>
       </c>
@@ -3634,7 +3651,7 @@
       </c>
       <c r="I49" s="32"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="30" t="s">
         <v>72</v>
       </c>
@@ -3659,7 +3676,7 @@
       </c>
       <c r="I50" s="32"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="30">
       <c r="A51" s="30" t="s">
         <v>73</v>
       </c>
@@ -3684,7 +3701,7 @@
       </c>
       <c r="I51" s="32"/>
     </row>
-    <row r="52" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="45">
       <c r="A52" s="30" t="s">
         <v>74</v>
       </c>
@@ -3709,7 +3726,7 @@
       </c>
       <c r="I52" s="32"/>
     </row>
-    <row r="53" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="45">
       <c r="A53" s="30" t="s">
         <v>75</v>
       </c>
@@ -3724,7 +3741,7 @@
         <v>19</v>
       </c>
       <c r="F53" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G53" s="30" t="s">
         <v>15</v>
@@ -3734,7 +3751,7 @@
       </c>
       <c r="I53" s="32"/>
     </row>
-    <row r="54" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="30" t="s">
         <v>76</v>
       </c>
@@ -3759,7 +3776,7 @@
       </c>
       <c r="I54" s="32"/>
     </row>
-    <row r="55" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="30">
       <c r="A55" s="30" t="s">
         <v>77</v>
       </c>
@@ -3784,7 +3801,7 @@
       </c>
       <c r="I55" s="32"/>
     </row>
-    <row r="56" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="45">
       <c r="A56" s="30" t="s">
         <v>78</v>
       </c>
@@ -3809,7 +3826,7 @@
       </c>
       <c r="I56" s="32"/>
     </row>
-    <row r="57" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="45">
       <c r="A57" s="30" t="s">
         <v>79</v>
       </c>
@@ -3834,7 +3851,7 @@
       </c>
       <c r="I57" s="32"/>
     </row>
-    <row r="58" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="30">
       <c r="A58" s="30" t="s">
         <v>80</v>
       </c>
@@ -3859,7 +3876,7 @@
       </c>
       <c r="I58" s="32"/>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="30">
       <c r="A59" s="30" t="s">
         <v>81</v>
       </c>
@@ -3884,7 +3901,7 @@
       </c>
       <c r="I59" s="32"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="30">
       <c r="A60" s="30" t="s">
         <v>82</v>
       </c>
@@ -3892,7 +3909,7 @@
         <v>176</v>
       </c>
       <c r="C60" s="32" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D60" s="30"/>
       <c r="E60" s="30" t="s">
@@ -3909,7 +3926,7 @@
       </c>
       <c r="I60" s="32"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="30">
       <c r="A61" s="30" t="s">
         <v>83</v>
       </c>
@@ -3917,7 +3934,7 @@
         <v>31</v>
       </c>
       <c r="C61" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D61" s="30"/>
       <c r="E61" s="30" t="s">
@@ -3934,7 +3951,7 @@
       </c>
       <c r="I61" s="32"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="45">
       <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
@@ -3959,7 +3976,7 @@
       </c>
       <c r="I62" s="32"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="45">
       <c r="A63" s="30" t="s">
         <v>85</v>
       </c>
@@ -3984,7 +4001,7 @@
       </c>
       <c r="I63" s="32"/>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="45">
       <c r="A64" s="30" t="s">
         <v>86</v>
       </c>
@@ -3995,7 +4012,7 @@
         <v>236</v>
       </c>
       <c r="D64" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E64" s="30" t="s">
         <v>19</v>
@@ -4011,7 +4028,7 @@
       </c>
       <c r="I64" s="32"/>
     </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="30">
       <c r="A65" s="30" t="s">
         <v>87</v>
       </c>
@@ -4022,7 +4039,7 @@
         <v>237</v>
       </c>
       <c r="D65" s="30" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E65" s="30" t="s">
         <v>19</v>
@@ -4038,7 +4055,7 @@
       </c>
       <c r="I65" s="32"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="30">
       <c r="A66" s="30" t="s">
         <v>88</v>
       </c>
@@ -4063,7 +4080,7 @@
       </c>
       <c r="I66" s="32"/>
     </row>
-    <row r="67" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="75">
       <c r="A67" s="30" t="s">
         <v>89</v>
       </c>
@@ -4088,7 +4105,7 @@
       </c>
       <c r="I67" s="32"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9">
       <c r="A68" s="30" t="s">
         <v>90</v>
       </c>
@@ -4113,7 +4130,7 @@
       </c>
       <c r="I68" s="32"/>
     </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="45">
       <c r="A69" s="30" t="s">
         <v>91</v>
       </c>
@@ -4138,7 +4155,7 @@
       </c>
       <c r="I69" s="32"/>
     </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="30">
       <c r="A70" s="30" t="s">
         <v>92</v>
       </c>
@@ -4163,7 +4180,7 @@
       </c>
       <c r="I70" s="32"/>
     </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="30">
       <c r="A71" s="30" t="s">
         <v>93</v>
       </c>
@@ -4188,7 +4205,7 @@
       </c>
       <c r="I71" s="32"/>
     </row>
-    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="30" t="s">
         <v>94</v>
       </c>
@@ -4213,7 +4230,7 @@
       </c>
       <c r="I72" s="32"/>
     </row>
-    <row r="73" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="30">
       <c r="A73" s="30" t="s">
         <v>95</v>
       </c>
@@ -4238,7 +4255,7 @@
       </c>
       <c r="I73" s="32"/>
     </row>
-    <row r="74" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="30">
       <c r="A74" s="30" t="s">
         <v>96</v>
       </c>
@@ -4263,7 +4280,7 @@
       </c>
       <c r="I74" s="32"/>
     </row>
-    <row r="75" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="30">
       <c r="A75" s="30" t="s">
         <v>97</v>
       </c>
@@ -4288,7 +4305,7 @@
       </c>
       <c r="I75" s="32"/>
     </row>
-    <row r="76" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="30">
       <c r="A76" s="30" t="s">
         <v>98</v>
       </c>
@@ -4313,7 +4330,7 @@
       </c>
       <c r="I76" s="32"/>
     </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="30">
       <c r="A77" s="30" t="s">
         <v>99</v>
       </c>
@@ -4338,7 +4355,7 @@
       </c>
       <c r="I77" s="32"/>
     </row>
-    <row r="78" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="135">
       <c r="A78" s="30" t="s">
         <v>100</v>
       </c>
@@ -4363,7 +4380,7 @@
       </c>
       <c r="I78" s="32"/>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="30">
       <c r="A79" s="30" t="s">
         <v>101</v>
       </c>
@@ -4388,7 +4405,7 @@
       </c>
       <c r="I79" s="32"/>
     </row>
-    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="30">
       <c r="A80" s="30" t="s">
         <v>102</v>
       </c>
@@ -4413,7 +4430,7 @@
       </c>
       <c r="I80" s="32"/>
     </row>
-    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="30" t="s">
         <v>103</v>
       </c>
@@ -4438,7 +4455,7 @@
       </c>
       <c r="I81" s="32"/>
     </row>
-    <row r="82" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="120">
       <c r="A82" s="30" t="s">
         <v>104</v>
       </c>
@@ -4463,7 +4480,7 @@
       </c>
       <c r="I82" s="32"/>
     </row>
-    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="30">
       <c r="A83" s="30" t="s">
         <v>105</v>
       </c>
@@ -4488,7 +4505,7 @@
       </c>
       <c r="I83" s="32"/>
     </row>
-    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="30">
       <c r="A84" s="30" t="s">
         <v>106</v>
       </c>
@@ -4513,7 +4530,7 @@
       </c>
       <c r="I84" s="32"/>
     </row>
-    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="30">
       <c r="A85" s="30" t="s">
         <v>107</v>
       </c>
@@ -4538,7 +4555,7 @@
       </c>
       <c r="I85" s="32"/>
     </row>
-    <row r="86" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="30">
       <c r="A86" s="30" t="s">
         <v>108</v>
       </c>
@@ -4563,7 +4580,7 @@
       </c>
       <c r="I86" s="32"/>
     </row>
-    <row r="87" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="120">
       <c r="A87" s="30" t="s">
         <v>109</v>
       </c>
@@ -4588,7 +4605,7 @@
       </c>
       <c r="I87" s="32"/>
     </row>
-    <row r="88" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="30">
       <c r="A88" s="30" t="s">
         <v>110</v>
       </c>
@@ -4613,7 +4630,7 @@
       </c>
       <c r="I88" s="32"/>
     </row>
-    <row r="89" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="60">
       <c r="A89" s="30" t="s">
         <v>111</v>
       </c>
@@ -4637,10 +4654,10 @@
         <v>17</v>
       </c>
       <c r="I89" s="20" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="30">
       <c r="A90" s="30" t="s">
         <v>112</v>
       </c>
@@ -4665,7 +4682,7 @@
       </c>
       <c r="I90" s="32"/>
     </row>
-    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="30">
       <c r="A91" s="30" t="s">
         <v>113</v>
       </c>
@@ -4690,7 +4707,7 @@
       </c>
       <c r="I91" s="32"/>
     </row>
-    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="45">
       <c r="A92" s="22" t="s">
         <v>114</v>
       </c>
@@ -4698,7 +4715,7 @@
         <v>184</v>
       </c>
       <c r="C92" s="20" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D92" s="30"/>
       <c r="E92" s="30" t="s">
@@ -4714,10 +4731,10 @@
         <v>17</v>
       </c>
       <c r="I92" s="20" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="30">
       <c r="A93" s="30" t="s">
         <v>115</v>
       </c>
@@ -4742,7 +4759,7 @@
       </c>
       <c r="I93" s="32"/>
     </row>
-    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="30">
       <c r="A94" s="30" t="s">
         <v>116</v>
       </c>
@@ -4767,7 +4784,7 @@
       </c>
       <c r="I94" s="32"/>
     </row>
-    <row r="95" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="120">
       <c r="A95" s="30" t="s">
         <v>117</v>
       </c>
@@ -4792,7 +4809,7 @@
       </c>
       <c r="I95" s="32"/>
     </row>
-    <row r="96" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="30">
       <c r="A96" s="30" t="s">
         <v>118</v>
       </c>
@@ -4817,7 +4834,7 @@
       </c>
       <c r="I96" s="32"/>
     </row>
-    <row r="97" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="30">
       <c r="A97" s="30" t="s">
         <v>119</v>
       </c>
@@ -4842,7 +4859,7 @@
       </c>
       <c r="I97" s="32"/>
     </row>
-    <row r="98" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="45">
       <c r="A98" s="30" t="s">
         <v>120</v>
       </c>
@@ -4867,7 +4884,7 @@
       </c>
       <c r="I98" s="32"/>
     </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="30">
       <c r="A99" s="30" t="s">
         <v>121</v>
       </c>
@@ -4878,7 +4895,7 @@
         <v>270</v>
       </c>
       <c r="D99" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E99" s="30" t="s">
         <v>19</v>
@@ -4894,7 +4911,7 @@
       </c>
       <c r="I99" s="32"/>
     </row>
-    <row r="100" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="45">
       <c r="A100" s="30" t="s">
         <v>122</v>
       </c>
@@ -4905,7 +4922,7 @@
         <v>271</v>
       </c>
       <c r="D100" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E100" s="30" t="s">
         <v>19</v>
@@ -4921,7 +4938,7 @@
       </c>
       <c r="I100" s="32"/>
     </row>
-    <row r="101" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="45">
       <c r="A101" s="30" t="s">
         <v>123</v>
       </c>
@@ -4932,7 +4949,7 @@
         <v>272</v>
       </c>
       <c r="D101" s="30" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E101" s="30" t="s">
         <v>19</v>
@@ -4948,15 +4965,15 @@
       </c>
       <c r="I101" s="20"/>
     </row>
-    <row r="102" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="60">
       <c r="A102" s="30" t="s">
         <v>124</v>
       </c>
       <c r="B102" s="31" t="s">
         <v>186</v>
       </c>
-      <c r="C102" s="32" t="s">
-        <v>273</v>
+      <c r="C102" s="20" t="s">
+        <v>345</v>
       </c>
       <c r="D102" s="30"/>
       <c r="E102" s="30" t="s">
@@ -4973,18 +4990,18 @@
       </c>
       <c r="I102" s="32"/>
     </row>
-    <row r="103" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A103" s="30" t="s">
+    <row r="103" spans="1:9" ht="45">
+      <c r="A103" s="22" t="s">
         <v>125</v>
       </c>
       <c r="B103" s="31" t="s">
         <v>186</v>
       </c>
       <c r="C103" s="32" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D103" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E103" s="30" t="s">
         <v>19</v>
@@ -5000,18 +5017,18 @@
       </c>
       <c r="I103" s="32"/>
     </row>
-    <row r="104" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="30" t="s">
+    <row r="104" spans="1:9" ht="30">
+      <c r="A104" s="22" t="s">
         <v>126</v>
       </c>
-      <c r="B104" s="31" t="s">
+      <c r="B104" s="24" t="s">
         <v>186</v>
       </c>
       <c r="C104" s="32" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D104" s="30" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E104" s="30" t="s">
         <v>19</v>
@@ -5027,7 +5044,7 @@
       </c>
       <c r="I104" s="32"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="30">
       <c r="A105" s="30" t="s">
         <v>127</v>
       </c>
@@ -5035,7 +5052,7 @@
         <v>32</v>
       </c>
       <c r="C105" s="32" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D105" s="30"/>
       <c r="E105" s="30" t="s">
@@ -5052,7 +5069,7 @@
       </c>
       <c r="I105" s="32"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="30">
       <c r="A106" s="30" t="s">
         <v>128</v>
       </c>
@@ -5060,10 +5077,10 @@
         <v>32</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D106" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E106" s="30" t="s">
         <v>19</v>
@@ -5079,7 +5096,7 @@
       </c>
       <c r="I106" s="32"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="30">
       <c r="A107" s="30" t="s">
         <v>129</v>
       </c>
@@ -5087,10 +5104,10 @@
         <v>32</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D107" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E107" s="30" t="s">
         <v>19</v>
@@ -5106,7 +5123,7 @@
       </c>
       <c r="I107" s="32"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="30" t="s">
         <v>130</v>
       </c>
@@ -5114,10 +5131,10 @@
         <v>32</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D108" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E108" s="30" t="s">
         <v>19</v>
@@ -5133,7 +5150,7 @@
       </c>
       <c r="I108" s="32"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="30">
       <c r="A109" s="30" t="s">
         <v>131</v>
       </c>
@@ -5141,16 +5158,16 @@
         <v>32</v>
       </c>
       <c r="C109" s="32" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D109" s="30" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E109" s="30" t="s">
         <v>19</v>
       </c>
       <c r="F109" s="30" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G109" s="30" t="s">
         <v>15</v>
@@ -5160,7 +5177,7 @@
       </c>
       <c r="I109" s="32"/>
     </row>
-    <row r="110" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="75">
       <c r="A110" s="30" t="s">
         <v>132</v>
       </c>
@@ -5168,7 +5185,7 @@
         <v>32</v>
       </c>
       <c r="C110" s="32" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D110" s="30"/>
       <c r="E110" s="30" t="s">
@@ -5185,7 +5202,7 @@
       </c>
       <c r="I110" s="32"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9">
       <c r="A111" s="30" t="s">
         <v>133</v>
       </c>
@@ -5193,7 +5210,7 @@
         <v>32</v>
       </c>
       <c r="C111" s="32" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D111" s="30"/>
       <c r="E111" s="30" t="s">
@@ -5210,7 +5227,7 @@
       </c>
       <c r="I111" s="32"/>
     </row>
-    <row r="112" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="30">
       <c r="A112" s="30" t="s">
         <v>134</v>
       </c>
@@ -5218,7 +5235,7 @@
         <v>32</v>
       </c>
       <c r="C112" s="32" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D112" s="30"/>
       <c r="E112" s="30" t="s">
@@ -5235,7 +5252,7 @@
       </c>
       <c r="I112" s="32"/>
     </row>
-    <row r="113" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="30">
       <c r="A113" s="30" t="s">
         <v>135</v>
       </c>
@@ -5260,7 +5277,7 @@
       </c>
       <c r="I113" s="32"/>
     </row>
-    <row r="114" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="30">
       <c r="A114" s="30" t="s">
         <v>136</v>
       </c>
@@ -5268,7 +5285,7 @@
         <v>188</v>
       </c>
       <c r="C114" s="32" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D114" s="30"/>
       <c r="E114" s="30" t="s">
@@ -5285,7 +5302,7 @@
       </c>
       <c r="I114" s="32"/>
     </row>
-    <row r="115" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="45">
       <c r="A115" s="30" t="s">
         <v>137</v>
       </c>
@@ -5293,7 +5310,7 @@
         <v>188</v>
       </c>
       <c r="C115" s="32" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D115" s="30"/>
       <c r="E115" s="30" t="s">
@@ -5310,7 +5327,7 @@
       </c>
       <c r="I115" s="32"/>
     </row>
-    <row r="116" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="30">
       <c r="A116" s="30" t="s">
         <v>138</v>
       </c>
@@ -5318,7 +5335,7 @@
         <v>188</v>
       </c>
       <c r="C116" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D116" s="30"/>
       <c r="E116" s="30" t="s">
@@ -5335,7 +5352,7 @@
       </c>
       <c r="I116" s="32"/>
     </row>
-    <row r="117" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="30">
       <c r="A117" s="30" t="s">
         <v>139</v>
       </c>
@@ -5343,7 +5360,7 @@
         <v>189</v>
       </c>
       <c r="C117" s="32" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D117" s="30"/>
       <c r="E117" s="30" t="s">
@@ -5360,7 +5377,7 @@
       </c>
       <c r="I117" s="32"/>
     </row>
-    <row r="118" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="30">
       <c r="A118" s="30" t="s">
         <v>140</v>
       </c>
@@ -5368,7 +5385,7 @@
         <v>189</v>
       </c>
       <c r="C118" s="32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D118" s="30"/>
       <c r="E118" s="30" t="s">
@@ -5385,7 +5402,7 @@
       </c>
       <c r="I118" s="32"/>
     </row>
-    <row r="119" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="30">
       <c r="A119" s="30" t="s">
         <v>141</v>
       </c>
@@ -5410,7 +5427,7 @@
       </c>
       <c r="I119" s="32"/>
     </row>
-    <row r="120" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="30">
       <c r="A120" s="30" t="s">
         <v>142</v>
       </c>
@@ -5418,7 +5435,7 @@
         <v>191</v>
       </c>
       <c r="C120" s="32" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D120" s="30"/>
       <c r="E120" s="30" t="s">
@@ -5435,7 +5452,7 @@
       </c>
       <c r="I120" s="32"/>
     </row>
-    <row r="121" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="60">
       <c r="A121" s="30" t="s">
         <v>143</v>
       </c>
@@ -5443,7 +5460,7 @@
         <v>191</v>
       </c>
       <c r="C121" s="32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D121" s="30"/>
       <c r="E121" s="30" t="s">
@@ -5460,7 +5477,7 @@
       </c>
       <c r="I121" s="32"/>
     </row>
-    <row r="122" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="30">
       <c r="A122" s="30" t="s">
         <v>144</v>
       </c>
@@ -5468,7 +5485,7 @@
         <v>192</v>
       </c>
       <c r="C122" s="32" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D122" s="30"/>
       <c r="E122" s="30" t="s">
@@ -5485,7 +5502,7 @@
       </c>
       <c r="I122" s="32"/>
     </row>
-    <row r="123" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="120">
       <c r="A123" s="30" t="s">
         <v>145</v>
       </c>
@@ -5493,7 +5510,7 @@
         <v>192</v>
       </c>
       <c r="C123" s="32" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D123" s="30"/>
       <c r="E123" s="30" t="s">
@@ -5510,7 +5527,7 @@
       </c>
       <c r="I123" s="32"/>
     </row>
-    <row r="124" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="30">
       <c r="A124" s="30" t="s">
         <v>146</v>
       </c>
@@ -5518,7 +5535,7 @@
         <v>192</v>
       </c>
       <c r="C124" s="32" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D124" s="30"/>
       <c r="E124" s="30" t="s">
@@ -5535,7 +5552,7 @@
       </c>
       <c r="I124" s="32"/>
     </row>
-    <row r="125" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="30" t="s">
         <v>147</v>
       </c>
@@ -5560,7 +5577,7 @@
       </c>
       <c r="I125" s="32"/>
     </row>
-    <row r="126" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="30">
       <c r="A126" s="30" t="s">
         <v>148</v>
       </c>
@@ -5568,7 +5585,7 @@
         <v>194</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D126" s="30"/>
       <c r="E126" s="30" t="s">
@@ -5585,7 +5602,7 @@
       </c>
       <c r="I126" s="32"/>
     </row>
-    <row r="127" spans="1:9" ht="135" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="135">
       <c r="A127" s="22" t="s">
         <v>149</v>
       </c>
@@ -5593,7 +5610,7 @@
         <v>194</v>
       </c>
       <c r="C127" s="32" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D127" s="30"/>
       <c r="E127" s="30" t="s">
@@ -5610,7 +5627,7 @@
       </c>
       <c r="I127" s="32"/>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="30">
       <c r="A128" s="30" t="s">
         <v>150</v>
       </c>
@@ -5618,7 +5635,7 @@
         <v>194</v>
       </c>
       <c r="C128" s="32" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D128" s="30"/>
       <c r="E128" s="30" t="s">
@@ -5635,7 +5652,7 @@
       </c>
       <c r="I128" s="32"/>
     </row>
-    <row r="129" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="45">
       <c r="A129" s="22" t="s">
         <v>151</v>
       </c>
@@ -5643,7 +5660,7 @@
         <v>194</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D129" s="30"/>
       <c r="E129" s="30" t="s">
@@ -5659,10 +5676,10 @@
         <v>17</v>
       </c>
       <c r="I129" s="20" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" ht="30">
       <c r="A130" s="30" t="s">
         <v>152</v>
       </c>
@@ -5670,7 +5687,7 @@
         <v>194</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D130" s="30"/>
       <c r="E130" s="30" t="s">
@@ -5687,7 +5704,7 @@
       </c>
       <c r="I130" s="32"/>
     </row>
-    <row r="131" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="30">
       <c r="A131" s="30" t="s">
         <v>153</v>
       </c>
@@ -5695,7 +5712,7 @@
         <v>194</v>
       </c>
       <c r="C131" s="32" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D131" s="30"/>
       <c r="E131" s="30" t="s">
@@ -5712,7 +5729,7 @@
       </c>
       <c r="I131" s="32"/>
     </row>
-    <row r="132" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" ht="30">
       <c r="A132" s="30" t="s">
         <v>154</v>
       </c>
@@ -5720,7 +5737,7 @@
         <v>194</v>
       </c>
       <c r="C132" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D132" s="30"/>
       <c r="E132" s="30" t="s">
@@ -5737,7 +5754,7 @@
       </c>
       <c r="I132" s="32"/>
     </row>
-    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="30">
       <c r="A133" s="30" t="s">
         <v>155</v>
       </c>
@@ -5745,7 +5762,7 @@
         <v>194</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D133" s="30"/>
       <c r="E133" s="30" t="s">
@@ -5762,7 +5779,7 @@
       </c>
       <c r="I133" s="32"/>
     </row>
-    <row r="134" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" ht="30">
       <c r="A134" s="30" t="s">
         <v>156</v>
       </c>
@@ -5770,7 +5787,7 @@
         <v>194</v>
       </c>
       <c r="C134" s="32" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D134" s="30"/>
       <c r="E134" s="30" t="s">
@@ -5787,7 +5804,7 @@
       </c>
       <c r="I134" s="32"/>
     </row>
-    <row r="135" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="45">
       <c r="A135" s="30" t="s">
         <v>157</v>
       </c>
@@ -5795,7 +5812,7 @@
         <v>194</v>
       </c>
       <c r="C135" s="32" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D135" s="30"/>
       <c r="E135" s="30" t="s">
@@ -5812,7 +5829,7 @@
       </c>
       <c r="I135" s="32"/>
     </row>
-    <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="45">
       <c r="A136" s="30" t="s">
         <v>158</v>
       </c>
@@ -5820,10 +5837,10 @@
         <v>195</v>
       </c>
       <c r="C136" s="32" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D136" s="30" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E136" s="30" t="s">
         <v>22</v>
@@ -5838,10 +5855,10 @@
         <v>21</v>
       </c>
       <c r="I136" s="32" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" ht="45">
       <c r="A137" s="30" t="s">
         <v>159</v>
       </c>
@@ -5849,7 +5866,7 @@
         <v>195</v>
       </c>
       <c r="C137" s="20" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D137" s="30"/>
       <c r="E137" s="30" t="s">
@@ -5866,7 +5883,7 @@
       </c>
       <c r="I137" s="32"/>
     </row>
-    <row r="138" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" ht="30">
       <c r="A138" s="30" t="s">
         <v>160</v>
       </c>
@@ -5874,7 +5891,7 @@
         <v>195</v>
       </c>
       <c r="C138" s="20" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D138" s="30"/>
       <c r="E138" s="30" t="s">
@@ -5891,7 +5908,7 @@
       </c>
       <c r="I138" s="32"/>
     </row>
-    <row r="139" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" ht="45">
       <c r="A139" s="30" t="s">
         <v>161</v>
       </c>
@@ -5899,10 +5916,10 @@
         <v>195</v>
       </c>
       <c r="C139" s="20" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D139" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E139" s="30" t="s">
         <v>22</v>
@@ -5917,10 +5934,10 @@
         <v>20</v>
       </c>
       <c r="I139" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" ht="45">
       <c r="A140" s="22" t="s">
         <v>162</v>
       </c>
@@ -5928,10 +5945,10 @@
         <v>195</v>
       </c>
       <c r="C140" s="20" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D140" s="30" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E140" s="30" t="s">
         <v>22</v>
@@ -5946,21 +5963,21 @@
         <v>20</v>
       </c>
       <c r="I140" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" ht="45">
       <c r="A141" s="22" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B141" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C141" s="20" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D141" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E141" s="33" t="s">
         <v>22</v>
@@ -5976,18 +5993,18 @@
       </c>
       <c r="I141" s="32"/>
     </row>
-    <row r="142" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" ht="60">
       <c r="A142" s="22" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B142" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C142" s="20" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D142" s="22" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E142" s="33" t="s">
         <v>22</v>
@@ -6002,48 +6019,50 @@
         <v>20</v>
       </c>
       <c r="I142" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" ht="60">
       <c r="A143" s="22" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="B143" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>333</v>
+        <v>343</v>
       </c>
       <c r="D143" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="E143" s="33" t="s">
+        <v>344</v>
+      </c>
+      <c r="E143" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="F143" s="30" t="s">
+      <c r="F143" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="G143" s="30" t="s">
+      <c r="G143" s="22" t="s">
         <v>15</v>
       </c>
       <c r="H143" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="I143" s="32"/>
-    </row>
-    <row r="144" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I143" s="20" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" ht="45">
       <c r="A144" s="22" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C144" s="20" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D144" s="22" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E144" s="33" t="s">
         <v>22</v>
@@ -6054,25 +6073,25 @@
       <c r="G144" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="H144" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="I144" s="32" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A145" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="B145" s="31" t="s">
+      <c r="H144" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="I144" s="32"/>
+    </row>
+    <row r="145" spans="1:9" ht="45">
+      <c r="A145" s="22" t="s">
+        <v>327</v>
+      </c>
+      <c r="B145" s="24" t="s">
         <v>195</v>
       </c>
       <c r="C145" s="20" t="s">
-        <v>335</v>
-      </c>
-      <c r="D145" s="30"/>
-      <c r="E145" s="30" t="s">
+        <v>333</v>
+      </c>
+      <c r="D145" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="E145" s="33" t="s">
         <v>22</v>
       </c>
       <c r="F145" s="30" t="s">
@@ -6082,17 +6101,44 @@
         <v>15</v>
       </c>
       <c r="H145" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="I145" s="32"/>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A146" s="3"/>
-      <c r="B146" s="10"/>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I145" s="32" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" ht="45">
+      <c r="A146" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="B146" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="C146" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="D146" s="30"/>
+      <c r="E146" s="30" t="s">
+        <v>22</v>
+      </c>
+      <c r="F146" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G146" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="H146" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="I146" s="32"/>
+    </row>
+    <row r="147" spans="1:9">
       <c r="A147" s="3"/>
       <c r="B147" s="10"/>
+    </row>
+    <row r="148" spans="1:9">
+      <c r="A148" s="3"/>
+      <c r="B148" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -6110,51 +6156,51 @@
     <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
-    <cfRule type="expression" dxfId="26" priority="53">
+  <conditionalFormatting sqref="A20:H74 I20:I104 A34:I146">
+    <cfRule type="expression" dxfId="7" priority="53">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="54">
+    <cfRule type="expression" dxfId="6" priority="54">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="61">
+    <cfRule type="expression" dxfId="5" priority="61">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A20:H74 I20:I145 A34:I145">
-    <cfRule type="expression" dxfId="23" priority="7">
+  <conditionalFormatting sqref="A20:H74 I20:I104 A34:I146">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F20:F145">
-    <cfRule type="expression" dxfId="20" priority="13">
+  <conditionalFormatting sqref="F20:F146">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F145" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F146" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E145" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E146" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G145" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G146" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H145" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H146" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6164,7 +6210,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B144:B147 B19:B143 C3" numberStoredAsText="1"/>
+    <ignoredError sqref="B144:B148 B19:B103 B105:B142" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -6255,12 +6301,12 @@
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{923F65C5-DEAB-400B-AA1F-124F40EE10AC}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>